<commit_message>
refactor: get product by size,color list & save data
</commit_message>
<xml_diff>
--- a/data/order_detail.xlsx
+++ b/data/order_detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\robot_test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFAB7DF-BADE-44F1-B7FE-86104F9252B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC88ECFB-5B61-4BC6-B462-55460F0C0639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E-commerce Sites" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Supplier Management</t>
   </si>
@@ -102,6 +102,18 @@
   <si>
     <t>000027065</t>
   </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>XS</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
 </sst>
 </file>
 
@@ -110,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;-&quot;mm&quot;-&quot;yyyy&quot; &quot;h&quot;:&quot;mm&quot;:&quot;ss"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -220,6 +232,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -259,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -341,6 +360,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -28605,7 +28625,7 @@
   <dimension ref="A1:E989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28696,36 +28716,36 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA199"/>
+  <dimension ref="A1:AC199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="19" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="34" customWidth="1"/>
-    <col min="4" max="5" width="15.5703125" style="34" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="34" customWidth="1"/>
-    <col min="7" max="16384" width="12.5703125" style="34"/>
+    <col min="3" max="3" width="18.28515625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15" style="19" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="34" customWidth="1"/>
+    <col min="6" max="7" width="15.5703125" style="34" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" style="34" customWidth="1"/>
+    <col min="9" max="16384" width="12.5703125" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="F1" s="21" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="H1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="26">
+      <c r="I1" s="26">
         <v>35</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
       <c r="J1" s="27"/>
       <c r="K1" s="27"/>
       <c r="L1" s="27"/>
@@ -28744,31 +28764,37 @@
       <c r="Y1" s="27"/>
       <c r="Z1" s="27"/>
       <c r="AA1" s="27"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
       <c r="L2" s="27"/>
@@ -28787,30 +28813,36 @@
       <c r="Y2" s="27"/>
       <c r="Z2" s="27"/>
       <c r="AA2" s="27"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="D3"/>
-      <c r="E3">
+      <c r="F3"/>
+      <c r="G3">
         <v>45</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
+      <c r="J3" s="28"/>
       <c r="K3" s="27"/>
       <c r="L3" s="27"/>
       <c r="M3" s="27"/>
@@ -28828,13 +28860,12 @@
       <c r="Y3" s="27"/>
       <c r="Z3" s="27"/>
       <c r="AA3" s="27"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB3" s="27"/>
+      <c r="AC3" s="27"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="J4" s="28"/>
       <c r="K4" s="27"/>
       <c r="L4" s="27"/>
       <c r="M4" s="27"/>
@@ -28852,13 +28883,15 @@
       <c r="Y4" s="27"/>
       <c r="Z4" s="27"/>
       <c r="AA4" s="27"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="27"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="24"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="J5" s="28"/>
       <c r="K5" s="27"/>
       <c r="L5" s="27"/>
       <c r="M5" s="27"/>
@@ -28876,13 +28909,15 @@
       <c r="Y5" s="27"/>
       <c r="Z5" s="27"/>
       <c r="AA5" s="27"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB5" s="27"/>
+      <c r="AC5" s="27"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="24"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="J6" s="28"/>
       <c r="K6" s="27"/>
       <c r="L6" s="27"/>
       <c r="M6" s="27"/>
@@ -28900,13 +28935,15 @@
       <c r="Y6" s="27"/>
       <c r="Z6" s="27"/>
       <c r="AA6" s="27"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB6" s="27"/>
+      <c r="AC6" s="27"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="24"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="J7" s="28"/>
       <c r="K7" s="27"/>
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
@@ -28924,13 +28961,15 @@
       <c r="Y7" s="27"/>
       <c r="Z7" s="27"/>
       <c r="AA7" s="27"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB7" s="27"/>
+      <c r="AC7" s="27"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="24"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="J8" s="28"/>
       <c r="K8" s="27"/>
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
@@ -28948,13 +28987,15 @@
       <c r="Y8" s="27"/>
       <c r="Z8" s="27"/>
       <c r="AA8" s="27"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="24"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="J9" s="28"/>
       <c r="K9" s="27"/>
       <c r="L9" s="27"/>
       <c r="M9" s="27"/>
@@ -28972,13 +29013,15 @@
       <c r="Y9" s="27"/>
       <c r="Z9" s="27"/>
       <c r="AA9" s="27"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="24"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="J10" s="28"/>
       <c r="K10" s="27"/>
       <c r="L10" s="27"/>
       <c r="M10" s="27"/>
@@ -28996,13 +29039,15 @@
       <c r="Y10" s="27"/>
       <c r="Z10" s="27"/>
       <c r="AA10" s="27"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB10" s="27"/>
+      <c r="AC10" s="27"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="J11" s="28"/>
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
@@ -29020,12 +29065,14 @@
       <c r="Y11" s="27"/>
       <c r="Z11" s="27"/>
       <c r="AA11" s="27"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB11" s="27"/>
+      <c r="AC11" s="27"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="24"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
       <c r="L12" s="27"/>
@@ -29044,10 +29091,10 @@
       <c r="Y12" s="27"/>
       <c r="Z12" s="27"/>
       <c r="AA12" s="27"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
+      <c r="AB12" s="27"/>
+      <c r="AC12" s="27"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
       <c r="L13" s="27"/>
@@ -29066,10 +29113,10 @@
       <c r="Y13" s="27"/>
       <c r="Z13" s="27"/>
       <c r="AA13" s="27"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
+      <c r="AB13" s="27"/>
+      <c r="AC13" s="27"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J14" s="27"/>
       <c r="K14" s="27"/>
       <c r="L14" s="27"/>
@@ -29088,10 +29135,10 @@
       <c r="Y14" s="27"/>
       <c r="Z14" s="27"/>
       <c r="AA14" s="27"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
+      <c r="AB14" s="27"/>
+      <c r="AC14" s="27"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
@@ -29110,10 +29157,10 @@
       <c r="Y15" s="27"/>
       <c r="Z15" s="27"/>
       <c r="AA15" s="27"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
+      <c r="AB15" s="27"/>
+      <c r="AC15" s="27"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J16" s="27"/>
       <c r="K16" s="27"/>
       <c r="L16" s="27"/>
@@ -29132,10 +29179,10 @@
       <c r="Y16" s="27"/>
       <c r="Z16" s="27"/>
       <c r="AA16" s="27"/>
-    </row>
-    <row r="17" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
+      <c r="AB16" s="27"/>
+      <c r="AC16" s="27"/>
+    </row>
+    <row r="17" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J17" s="27"/>
       <c r="K17" s="27"/>
       <c r="L17" s="27"/>
@@ -29154,10 +29201,10 @@
       <c r="Y17" s="27"/>
       <c r="Z17" s="27"/>
       <c r="AA17" s="27"/>
-    </row>
-    <row r="18" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
+      <c r="AB17" s="27"/>
+      <c r="AC17" s="27"/>
+    </row>
+    <row r="18" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J18" s="27"/>
       <c r="K18" s="27"/>
       <c r="L18" s="27"/>
@@ -29176,10 +29223,10 @@
       <c r="Y18" s="27"/>
       <c r="Z18" s="27"/>
       <c r="AA18" s="27"/>
-    </row>
-    <row r="19" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
+      <c r="AB18" s="27"/>
+      <c r="AC18" s="27"/>
+    </row>
+    <row r="19" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J19" s="27"/>
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
@@ -29198,10 +29245,10 @@
       <c r="Y19" s="27"/>
       <c r="Z19" s="27"/>
       <c r="AA19" s="27"/>
-    </row>
-    <row r="20" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
+      <c r="AB19" s="27"/>
+      <c r="AC19" s="27"/>
+    </row>
+    <row r="20" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J20" s="27"/>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
@@ -29220,10 +29267,10 @@
       <c r="Y20" s="27"/>
       <c r="Z20" s="27"/>
       <c r="AA20" s="27"/>
-    </row>
-    <row r="21" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
+      <c r="AB20" s="27"/>
+      <c r="AC20" s="27"/>
+    </row>
+    <row r="21" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
@@ -29242,10 +29289,10 @@
       <c r="Y21" s="27"/>
       <c r="Z21" s="27"/>
       <c r="AA21" s="27"/>
-    </row>
-    <row r="22" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
+      <c r="AB21" s="27"/>
+      <c r="AC21" s="27"/>
+    </row>
+    <row r="22" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J22" s="27"/>
       <c r="K22" s="27"/>
       <c r="L22" s="27"/>
@@ -29264,10 +29311,10 @@
       <c r="Y22" s="27"/>
       <c r="Z22" s="27"/>
       <c r="AA22" s="27"/>
-    </row>
-    <row r="23" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
+      <c r="AB22" s="27"/>
+      <c r="AC22" s="27"/>
+    </row>
+    <row r="23" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J23" s="27"/>
       <c r="K23" s="27"/>
       <c r="L23" s="27"/>
@@ -29286,10 +29333,10 @@
       <c r="Y23" s="27"/>
       <c r="Z23" s="27"/>
       <c r="AA23" s="27"/>
-    </row>
-    <row r="24" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
+      <c r="AB23" s="27"/>
+      <c r="AC23" s="27"/>
+    </row>
+    <row r="24" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J24" s="27"/>
       <c r="K24" s="27"/>
       <c r="L24" s="27"/>
@@ -29308,10 +29355,10 @@
       <c r="Y24" s="27"/>
       <c r="Z24" s="27"/>
       <c r="AA24" s="27"/>
-    </row>
-    <row r="25" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
+      <c r="AB24" s="27"/>
+      <c r="AC24" s="27"/>
+    </row>
+    <row r="25" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J25" s="27"/>
       <c r="K25" s="27"/>
       <c r="L25" s="27"/>
@@ -29330,10 +29377,10 @@
       <c r="Y25" s="27"/>
       <c r="Z25" s="27"/>
       <c r="AA25" s="27"/>
-    </row>
-    <row r="26" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
+      <c r="AB25" s="27"/>
+      <c r="AC25" s="27"/>
+    </row>
+    <row r="26" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
@@ -29352,10 +29399,10 @@
       <c r="Y26" s="27"/>
       <c r="Z26" s="27"/>
       <c r="AA26" s="27"/>
-    </row>
-    <row r="27" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
+      <c r="AB26" s="27"/>
+      <c r="AC26" s="27"/>
+    </row>
+    <row r="27" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J27" s="27"/>
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
@@ -29374,10 +29421,10 @@
       <c r="Y27" s="27"/>
       <c r="Z27" s="27"/>
       <c r="AA27" s="27"/>
-    </row>
-    <row r="28" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
+      <c r="AB27" s="27"/>
+      <c r="AC27" s="27"/>
+    </row>
+    <row r="28" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J28" s="27"/>
       <c r="K28" s="27"/>
       <c r="L28" s="27"/>
@@ -29396,10 +29443,10 @@
       <c r="Y28" s="27"/>
       <c r="Z28" s="27"/>
       <c r="AA28" s="27"/>
-    </row>
-    <row r="29" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
+      <c r="AB28" s="27"/>
+      <c r="AC28" s="27"/>
+    </row>
+    <row r="29" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
@@ -29418,10 +29465,10 @@
       <c r="Y29" s="27"/>
       <c r="Z29" s="27"/>
       <c r="AA29" s="27"/>
-    </row>
-    <row r="30" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
+      <c r="AB29" s="27"/>
+      <c r="AC29" s="27"/>
+    </row>
+    <row r="30" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>
@@ -29440,10 +29487,10 @@
       <c r="Y30" s="27"/>
       <c r="Z30" s="27"/>
       <c r="AA30" s="27"/>
-    </row>
-    <row r="31" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
+      <c r="AB30" s="27"/>
+      <c r="AC30" s="27"/>
+    </row>
+    <row r="31" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J31" s="27"/>
       <c r="K31" s="27"/>
       <c r="L31" s="27"/>
@@ -29462,10 +29509,10 @@
       <c r="Y31" s="27"/>
       <c r="Z31" s="27"/>
       <c r="AA31" s="27"/>
-    </row>
-    <row r="32" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
+      <c r="AB31" s="27"/>
+      <c r="AC31" s="27"/>
+    </row>
+    <row r="32" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J32" s="27"/>
       <c r="K32" s="27"/>
       <c r="L32" s="27"/>
@@ -29484,10 +29531,10 @@
       <c r="Y32" s="27"/>
       <c r="Z32" s="27"/>
       <c r="AA32" s="27"/>
-    </row>
-    <row r="33" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
+      <c r="AB32" s="27"/>
+      <c r="AC32" s="27"/>
+    </row>
+    <row r="33" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J33" s="27"/>
       <c r="K33" s="27"/>
       <c r="L33" s="27"/>
@@ -29506,10 +29553,10 @@
       <c r="Y33" s="27"/>
       <c r="Z33" s="27"/>
       <c r="AA33" s="27"/>
-    </row>
-    <row r="34" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
+      <c r="AB33" s="27"/>
+      <c r="AC33" s="27"/>
+    </row>
+    <row r="34" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J34" s="27"/>
       <c r="K34" s="27"/>
       <c r="L34" s="27"/>
@@ -29528,10 +29575,10 @@
       <c r="Y34" s="27"/>
       <c r="Z34" s="27"/>
       <c r="AA34" s="27"/>
-    </row>
-    <row r="35" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
+      <c r="AB34" s="27"/>
+      <c r="AC34" s="27"/>
+    </row>
+    <row r="35" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J35" s="27"/>
       <c r="K35" s="27"/>
       <c r="L35" s="27"/>
@@ -29550,10 +29597,10 @@
       <c r="Y35" s="27"/>
       <c r="Z35" s="27"/>
       <c r="AA35" s="27"/>
-    </row>
-    <row r="36" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
+      <c r="AB35" s="27"/>
+      <c r="AC35" s="27"/>
+    </row>
+    <row r="36" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J36" s="27"/>
       <c r="K36" s="27"/>
       <c r="L36" s="27"/>
@@ -29572,10 +29619,10 @@
       <c r="Y36" s="27"/>
       <c r="Z36" s="27"/>
       <c r="AA36" s="27"/>
-    </row>
-    <row r="37" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
+      <c r="AB36" s="27"/>
+      <c r="AC36" s="27"/>
+    </row>
+    <row r="37" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J37" s="27"/>
       <c r="K37" s="27"/>
       <c r="L37" s="27"/>
@@ -29594,10 +29641,10 @@
       <c r="Y37" s="27"/>
       <c r="Z37" s="27"/>
       <c r="AA37" s="27"/>
-    </row>
-    <row r="38" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
+      <c r="AB37" s="27"/>
+      <c r="AC37" s="27"/>
+    </row>
+    <row r="38" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J38" s="27"/>
       <c r="K38" s="27"/>
       <c r="L38" s="27"/>
@@ -29616,10 +29663,10 @@
       <c r="Y38" s="27"/>
       <c r="Z38" s="27"/>
       <c r="AA38" s="27"/>
-    </row>
-    <row r="39" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
+      <c r="AB38" s="27"/>
+      <c r="AC38" s="27"/>
+    </row>
+    <row r="39" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J39" s="27"/>
       <c r="K39" s="27"/>
       <c r="L39" s="27"/>
@@ -29638,10 +29685,10 @@
       <c r="Y39" s="27"/>
       <c r="Z39" s="27"/>
       <c r="AA39" s="27"/>
-    </row>
-    <row r="40" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
+      <c r="AB39" s="27"/>
+      <c r="AC39" s="27"/>
+    </row>
+    <row r="40" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J40" s="27"/>
       <c r="K40" s="27"/>
       <c r="L40" s="27"/>
@@ -29660,10 +29707,10 @@
       <c r="Y40" s="27"/>
       <c r="Z40" s="27"/>
       <c r="AA40" s="27"/>
-    </row>
-    <row r="41" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
+      <c r="AB40" s="27"/>
+      <c r="AC40" s="27"/>
+    </row>
+    <row r="41" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J41" s="27"/>
       <c r="K41" s="27"/>
       <c r="L41" s="27"/>
@@ -29682,10 +29729,10 @@
       <c r="Y41" s="27"/>
       <c r="Z41" s="27"/>
       <c r="AA41" s="27"/>
-    </row>
-    <row r="42" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
+      <c r="AB41" s="27"/>
+      <c r="AC41" s="27"/>
+    </row>
+    <row r="42" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J42" s="27"/>
       <c r="K42" s="27"/>
       <c r="L42" s="27"/>
@@ -29704,10 +29751,10 @@
       <c r="Y42" s="27"/>
       <c r="Z42" s="27"/>
       <c r="AA42" s="27"/>
-    </row>
-    <row r="43" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
+      <c r="AB42" s="27"/>
+      <c r="AC42" s="27"/>
+    </row>
+    <row r="43" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J43" s="27"/>
       <c r="K43" s="27"/>
       <c r="L43" s="27"/>
@@ -29726,10 +29773,10 @@
       <c r="Y43" s="27"/>
       <c r="Z43" s="27"/>
       <c r="AA43" s="27"/>
-    </row>
-    <row r="44" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
+      <c r="AB43" s="27"/>
+      <c r="AC43" s="27"/>
+    </row>
+    <row r="44" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J44" s="27"/>
       <c r="K44" s="27"/>
       <c r="L44" s="27"/>
@@ -29748,10 +29795,10 @@
       <c r="Y44" s="27"/>
       <c r="Z44" s="27"/>
       <c r="AA44" s="27"/>
-    </row>
-    <row r="45" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
+      <c r="AB44" s="27"/>
+      <c r="AC44" s="27"/>
+    </row>
+    <row r="45" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J45" s="27"/>
       <c r="K45" s="27"/>
       <c r="L45" s="27"/>
@@ -29770,10 +29817,10 @@
       <c r="Y45" s="27"/>
       <c r="Z45" s="27"/>
       <c r="AA45" s="27"/>
-    </row>
-    <row r="46" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
+      <c r="AB45" s="27"/>
+      <c r="AC45" s="27"/>
+    </row>
+    <row r="46" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J46" s="27"/>
       <c r="K46" s="27"/>
       <c r="L46" s="27"/>
@@ -29792,10 +29839,10 @@
       <c r="Y46" s="27"/>
       <c r="Z46" s="27"/>
       <c r="AA46" s="27"/>
-    </row>
-    <row r="47" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
+      <c r="AB46" s="27"/>
+      <c r="AC46" s="27"/>
+    </row>
+    <row r="47" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J47" s="27"/>
       <c r="K47" s="27"/>
       <c r="L47" s="27"/>
@@ -29814,10 +29861,10 @@
       <c r="Y47" s="27"/>
       <c r="Z47" s="27"/>
       <c r="AA47" s="27"/>
-    </row>
-    <row r="48" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
+      <c r="AB47" s="27"/>
+      <c r="AC47" s="27"/>
+    </row>
+    <row r="48" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J48" s="27"/>
       <c r="K48" s="27"/>
       <c r="L48" s="27"/>
@@ -29836,10 +29883,10 @@
       <c r="Y48" s="27"/>
       <c r="Z48" s="27"/>
       <c r="AA48" s="27"/>
-    </row>
-    <row r="49" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
+      <c r="AB48" s="27"/>
+      <c r="AC48" s="27"/>
+    </row>
+    <row r="49" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J49" s="27"/>
       <c r="K49" s="27"/>
       <c r="L49" s="27"/>
@@ -29858,10 +29905,10 @@
       <c r="Y49" s="27"/>
       <c r="Z49" s="27"/>
       <c r="AA49" s="27"/>
-    </row>
-    <row r="50" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
+      <c r="AB49" s="27"/>
+      <c r="AC49" s="27"/>
+    </row>
+    <row r="50" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J50" s="27"/>
       <c r="K50" s="27"/>
       <c r="L50" s="27"/>
@@ -29880,10 +29927,10 @@
       <c r="Y50" s="27"/>
       <c r="Z50" s="27"/>
       <c r="AA50" s="27"/>
-    </row>
-    <row r="51" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
+      <c r="AB50" s="27"/>
+      <c r="AC50" s="27"/>
+    </row>
+    <row r="51" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J51" s="27"/>
       <c r="K51" s="27"/>
       <c r="L51" s="27"/>
@@ -29902,10 +29949,10 @@
       <c r="Y51" s="27"/>
       <c r="Z51" s="27"/>
       <c r="AA51" s="27"/>
-    </row>
-    <row r="52" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
+      <c r="AB51" s="27"/>
+      <c r="AC51" s="27"/>
+    </row>
+    <row r="52" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J52" s="27"/>
       <c r="K52" s="27"/>
       <c r="L52" s="27"/>
@@ -29924,10 +29971,10 @@
       <c r="Y52" s="27"/>
       <c r="Z52" s="27"/>
       <c r="AA52" s="27"/>
-    </row>
-    <row r="53" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
+      <c r="AB52" s="27"/>
+      <c r="AC52" s="27"/>
+    </row>
+    <row r="53" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J53" s="27"/>
       <c r="K53" s="27"/>
       <c r="L53" s="27"/>
@@ -29946,10 +29993,10 @@
       <c r="Y53" s="27"/>
       <c r="Z53" s="27"/>
       <c r="AA53" s="27"/>
-    </row>
-    <row r="54" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H54" s="27"/>
-      <c r="I54" s="27"/>
+      <c r="AB53" s="27"/>
+      <c r="AC53" s="27"/>
+    </row>
+    <row r="54" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J54" s="27"/>
       <c r="K54" s="27"/>
       <c r="L54" s="27"/>
@@ -29968,10 +30015,10 @@
       <c r="Y54" s="27"/>
       <c r="Z54" s="27"/>
       <c r="AA54" s="27"/>
-    </row>
-    <row r="55" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H55" s="27"/>
-      <c r="I55" s="27"/>
+      <c r="AB54" s="27"/>
+      <c r="AC54" s="27"/>
+    </row>
+    <row r="55" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J55" s="27"/>
       <c r="K55" s="27"/>
       <c r="L55" s="27"/>
@@ -29990,10 +30037,10 @@
       <c r="Y55" s="27"/>
       <c r="Z55" s="27"/>
       <c r="AA55" s="27"/>
-    </row>
-    <row r="56" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
+      <c r="AB55" s="27"/>
+      <c r="AC55" s="27"/>
+    </row>
+    <row r="56" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J56" s="27"/>
       <c r="K56" s="27"/>
       <c r="L56" s="27"/>
@@ -30012,10 +30059,10 @@
       <c r="Y56" s="27"/>
       <c r="Z56" s="27"/>
       <c r="AA56" s="27"/>
-    </row>
-    <row r="57" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H57" s="27"/>
-      <c r="I57" s="27"/>
+      <c r="AB56" s="27"/>
+      <c r="AC56" s="27"/>
+    </row>
+    <row r="57" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J57" s="27"/>
       <c r="K57" s="27"/>
       <c r="L57" s="27"/>
@@ -30034,10 +30081,10 @@
       <c r="Y57" s="27"/>
       <c r="Z57" s="27"/>
       <c r="AA57" s="27"/>
-    </row>
-    <row r="58" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H58" s="27"/>
-      <c r="I58" s="27"/>
+      <c r="AB57" s="27"/>
+      <c r="AC57" s="27"/>
+    </row>
+    <row r="58" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J58" s="27"/>
       <c r="K58" s="27"/>
       <c r="L58" s="27"/>
@@ -30056,10 +30103,10 @@
       <c r="Y58" s="27"/>
       <c r="Z58" s="27"/>
       <c r="AA58" s="27"/>
-    </row>
-    <row r="59" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H59" s="27"/>
-      <c r="I59" s="27"/>
+      <c r="AB58" s="27"/>
+      <c r="AC58" s="27"/>
+    </row>
+    <row r="59" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J59" s="27"/>
       <c r="K59" s="27"/>
       <c r="L59" s="27"/>
@@ -30078,10 +30125,10 @@
       <c r="Y59" s="27"/>
       <c r="Z59" s="27"/>
       <c r="AA59" s="27"/>
-    </row>
-    <row r="60" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H60" s="27"/>
-      <c r="I60" s="27"/>
+      <c r="AB59" s="27"/>
+      <c r="AC59" s="27"/>
+    </row>
+    <row r="60" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J60" s="27"/>
       <c r="K60" s="27"/>
       <c r="L60" s="27"/>
@@ -30100,10 +30147,10 @@
       <c r="Y60" s="27"/>
       <c r="Z60" s="27"/>
       <c r="AA60" s="27"/>
-    </row>
-    <row r="61" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H61" s="27"/>
-      <c r="I61" s="27"/>
+      <c r="AB60" s="27"/>
+      <c r="AC60" s="27"/>
+    </row>
+    <row r="61" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J61" s="27"/>
       <c r="K61" s="27"/>
       <c r="L61" s="27"/>
@@ -30122,10 +30169,10 @@
       <c r="Y61" s="27"/>
       <c r="Z61" s="27"/>
       <c r="AA61" s="27"/>
-    </row>
-    <row r="62" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H62" s="27"/>
-      <c r="I62" s="27"/>
+      <c r="AB61" s="27"/>
+      <c r="AC61" s="27"/>
+    </row>
+    <row r="62" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J62" s="27"/>
       <c r="K62" s="27"/>
       <c r="L62" s="27"/>
@@ -30144,10 +30191,10 @@
       <c r="Y62" s="27"/>
       <c r="Z62" s="27"/>
       <c r="AA62" s="27"/>
-    </row>
-    <row r="63" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H63" s="27"/>
-      <c r="I63" s="27"/>
+      <c r="AB62" s="27"/>
+      <c r="AC62" s="27"/>
+    </row>
+    <row r="63" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J63" s="27"/>
       <c r="K63" s="27"/>
       <c r="L63" s="27"/>
@@ -30166,10 +30213,10 @@
       <c r="Y63" s="27"/>
       <c r="Z63" s="27"/>
       <c r="AA63" s="27"/>
-    </row>
-    <row r="64" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H64" s="27"/>
-      <c r="I64" s="27"/>
+      <c r="AB63" s="27"/>
+      <c r="AC63" s="27"/>
+    </row>
+    <row r="64" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J64" s="27"/>
       <c r="K64" s="27"/>
       <c r="L64" s="27"/>
@@ -30188,10 +30235,10 @@
       <c r="Y64" s="27"/>
       <c r="Z64" s="27"/>
       <c r="AA64" s="27"/>
-    </row>
-    <row r="65" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H65" s="27"/>
-      <c r="I65" s="27"/>
+      <c r="AB64" s="27"/>
+      <c r="AC64" s="27"/>
+    </row>
+    <row r="65" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J65" s="27"/>
       <c r="K65" s="27"/>
       <c r="L65" s="27"/>
@@ -30210,10 +30257,10 @@
       <c r="Y65" s="27"/>
       <c r="Z65" s="27"/>
       <c r="AA65" s="27"/>
-    </row>
-    <row r="66" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H66" s="27"/>
-      <c r="I66" s="27"/>
+      <c r="AB65" s="27"/>
+      <c r="AC65" s="27"/>
+    </row>
+    <row r="66" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J66" s="27"/>
       <c r="K66" s="27"/>
       <c r="L66" s="27"/>
@@ -30232,10 +30279,10 @@
       <c r="Y66" s="27"/>
       <c r="Z66" s="27"/>
       <c r="AA66" s="27"/>
-    </row>
-    <row r="67" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H67" s="27"/>
-      <c r="I67" s="27"/>
+      <c r="AB66" s="27"/>
+      <c r="AC66" s="27"/>
+    </row>
+    <row r="67" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J67" s="27"/>
       <c r="K67" s="27"/>
       <c r="L67" s="27"/>
@@ -30254,10 +30301,10 @@
       <c r="Y67" s="27"/>
       <c r="Z67" s="27"/>
       <c r="AA67" s="27"/>
-    </row>
-    <row r="68" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H68" s="27"/>
-      <c r="I68" s="27"/>
+      <c r="AB67" s="27"/>
+      <c r="AC67" s="27"/>
+    </row>
+    <row r="68" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J68" s="27"/>
       <c r="K68" s="27"/>
       <c r="L68" s="27"/>
@@ -30276,10 +30323,10 @@
       <c r="Y68" s="27"/>
       <c r="Z68" s="27"/>
       <c r="AA68" s="27"/>
-    </row>
-    <row r="69" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H69" s="27"/>
-      <c r="I69" s="27"/>
+      <c r="AB68" s="27"/>
+      <c r="AC68" s="27"/>
+    </row>
+    <row r="69" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J69" s="27"/>
       <c r="K69" s="27"/>
       <c r="L69" s="27"/>
@@ -30298,10 +30345,10 @@
       <c r="Y69" s="27"/>
       <c r="Z69" s="27"/>
       <c r="AA69" s="27"/>
-    </row>
-    <row r="70" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H70" s="27"/>
-      <c r="I70" s="27"/>
+      <c r="AB69" s="27"/>
+      <c r="AC69" s="27"/>
+    </row>
+    <row r="70" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J70" s="27"/>
       <c r="K70" s="27"/>
       <c r="L70" s="27"/>
@@ -30320,10 +30367,10 @@
       <c r="Y70" s="27"/>
       <c r="Z70" s="27"/>
       <c r="AA70" s="27"/>
-    </row>
-    <row r="71" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H71" s="27"/>
-      <c r="I71" s="27"/>
+      <c r="AB70" s="27"/>
+      <c r="AC70" s="27"/>
+    </row>
+    <row r="71" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J71" s="27"/>
       <c r="K71" s="27"/>
       <c r="L71" s="27"/>
@@ -30342,10 +30389,10 @@
       <c r="Y71" s="27"/>
       <c r="Z71" s="27"/>
       <c r="AA71" s="27"/>
-    </row>
-    <row r="72" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H72" s="27"/>
-      <c r="I72" s="27"/>
+      <c r="AB71" s="27"/>
+      <c r="AC71" s="27"/>
+    </row>
+    <row r="72" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J72" s="27"/>
       <c r="K72" s="27"/>
       <c r="L72" s="27"/>
@@ -30364,10 +30411,10 @@
       <c r="Y72" s="27"/>
       <c r="Z72" s="27"/>
       <c r="AA72" s="27"/>
-    </row>
-    <row r="73" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H73" s="27"/>
-      <c r="I73" s="27"/>
+      <c r="AB72" s="27"/>
+      <c r="AC72" s="27"/>
+    </row>
+    <row r="73" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J73" s="27"/>
       <c r="K73" s="27"/>
       <c r="L73" s="27"/>
@@ -30386,10 +30433,10 @@
       <c r="Y73" s="27"/>
       <c r="Z73" s="27"/>
       <c r="AA73" s="27"/>
-    </row>
-    <row r="74" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H74" s="27"/>
-      <c r="I74" s="27"/>
+      <c r="AB73" s="27"/>
+      <c r="AC73" s="27"/>
+    </row>
+    <row r="74" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J74" s="27"/>
       <c r="K74" s="27"/>
       <c r="L74" s="27"/>
@@ -30408,10 +30455,10 @@
       <c r="Y74" s="27"/>
       <c r="Z74" s="27"/>
       <c r="AA74" s="27"/>
-    </row>
-    <row r="75" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H75" s="27"/>
-      <c r="I75" s="27"/>
+      <c r="AB74" s="27"/>
+      <c r="AC74" s="27"/>
+    </row>
+    <row r="75" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J75" s="27"/>
       <c r="K75" s="27"/>
       <c r="L75" s="27"/>
@@ -30430,10 +30477,10 @@
       <c r="Y75" s="27"/>
       <c r="Z75" s="27"/>
       <c r="AA75" s="27"/>
-    </row>
-    <row r="76" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H76" s="27"/>
-      <c r="I76" s="27"/>
+      <c r="AB75" s="27"/>
+      <c r="AC75" s="27"/>
+    </row>
+    <row r="76" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J76" s="27"/>
       <c r="K76" s="27"/>
       <c r="L76" s="27"/>
@@ -30452,10 +30499,10 @@
       <c r="Y76" s="27"/>
       <c r="Z76" s="27"/>
       <c r="AA76" s="27"/>
-    </row>
-    <row r="77" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H77" s="27"/>
-      <c r="I77" s="27"/>
+      <c r="AB76" s="27"/>
+      <c r="AC76" s="27"/>
+    </row>
+    <row r="77" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J77" s="27"/>
       <c r="K77" s="27"/>
       <c r="L77" s="27"/>
@@ -30474,10 +30521,10 @@
       <c r="Y77" s="27"/>
       <c r="Z77" s="27"/>
       <c r="AA77" s="27"/>
-    </row>
-    <row r="78" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H78" s="27"/>
-      <c r="I78" s="27"/>
+      <c r="AB77" s="27"/>
+      <c r="AC77" s="27"/>
+    </row>
+    <row r="78" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J78" s="27"/>
       <c r="K78" s="27"/>
       <c r="L78" s="27"/>
@@ -30496,10 +30543,10 @@
       <c r="Y78" s="27"/>
       <c r="Z78" s="27"/>
       <c r="AA78" s="27"/>
-    </row>
-    <row r="79" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H79" s="27"/>
-      <c r="I79" s="27"/>
+      <c r="AB78" s="27"/>
+      <c r="AC78" s="27"/>
+    </row>
+    <row r="79" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J79" s="27"/>
       <c r="K79" s="27"/>
       <c r="L79" s="27"/>
@@ -30518,10 +30565,10 @@
       <c r="Y79" s="27"/>
       <c r="Z79" s="27"/>
       <c r="AA79" s="27"/>
-    </row>
-    <row r="80" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H80" s="27"/>
-      <c r="I80" s="27"/>
+      <c r="AB79" s="27"/>
+      <c r="AC79" s="27"/>
+    </row>
+    <row r="80" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J80" s="27"/>
       <c r="K80" s="27"/>
       <c r="L80" s="27"/>
@@ -30540,10 +30587,10 @@
       <c r="Y80" s="27"/>
       <c r="Z80" s="27"/>
       <c r="AA80" s="27"/>
-    </row>
-    <row r="81" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H81" s="27"/>
-      <c r="I81" s="27"/>
+      <c r="AB80" s="27"/>
+      <c r="AC80" s="27"/>
+    </row>
+    <row r="81" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J81" s="27"/>
       <c r="K81" s="27"/>
       <c r="L81" s="27"/>
@@ -30562,10 +30609,10 @@
       <c r="Y81" s="27"/>
       <c r="Z81" s="27"/>
       <c r="AA81" s="27"/>
-    </row>
-    <row r="82" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H82" s="27"/>
-      <c r="I82" s="27"/>
+      <c r="AB81" s="27"/>
+      <c r="AC81" s="27"/>
+    </row>
+    <row r="82" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J82" s="27"/>
       <c r="K82" s="27"/>
       <c r="L82" s="27"/>
@@ -30584,10 +30631,10 @@
       <c r="Y82" s="27"/>
       <c r="Z82" s="27"/>
       <c r="AA82" s="27"/>
-    </row>
-    <row r="83" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H83" s="27"/>
-      <c r="I83" s="27"/>
+      <c r="AB82" s="27"/>
+      <c r="AC82" s="27"/>
+    </row>
+    <row r="83" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J83" s="27"/>
       <c r="K83" s="27"/>
       <c r="L83" s="27"/>
@@ -30606,10 +30653,10 @@
       <c r="Y83" s="27"/>
       <c r="Z83" s="27"/>
       <c r="AA83" s="27"/>
-    </row>
-    <row r="84" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H84" s="27"/>
-      <c r="I84" s="27"/>
+      <c r="AB83" s="27"/>
+      <c r="AC83" s="27"/>
+    </row>
+    <row r="84" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J84" s="27"/>
       <c r="K84" s="27"/>
       <c r="L84" s="27"/>
@@ -30628,10 +30675,10 @@
       <c r="Y84" s="27"/>
       <c r="Z84" s="27"/>
       <c r="AA84" s="27"/>
-    </row>
-    <row r="85" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H85" s="27"/>
-      <c r="I85" s="27"/>
+      <c r="AB84" s="27"/>
+      <c r="AC84" s="27"/>
+    </row>
+    <row r="85" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J85" s="27"/>
       <c r="K85" s="27"/>
       <c r="L85" s="27"/>
@@ -30650,10 +30697,10 @@
       <c r="Y85" s="27"/>
       <c r="Z85" s="27"/>
       <c r="AA85" s="27"/>
-    </row>
-    <row r="86" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H86" s="27"/>
-      <c r="I86" s="27"/>
+      <c r="AB85" s="27"/>
+      <c r="AC85" s="27"/>
+    </row>
+    <row r="86" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J86" s="27"/>
       <c r="K86" s="27"/>
       <c r="L86" s="27"/>
@@ -30672,10 +30719,10 @@
       <c r="Y86" s="27"/>
       <c r="Z86" s="27"/>
       <c r="AA86" s="27"/>
-    </row>
-    <row r="87" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H87" s="27"/>
-      <c r="I87" s="27"/>
+      <c r="AB86" s="27"/>
+      <c r="AC86" s="27"/>
+    </row>
+    <row r="87" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J87" s="27"/>
       <c r="K87" s="27"/>
       <c r="L87" s="27"/>
@@ -30694,10 +30741,10 @@
       <c r="Y87" s="27"/>
       <c r="Z87" s="27"/>
       <c r="AA87" s="27"/>
-    </row>
-    <row r="88" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H88" s="27"/>
-      <c r="I88" s="27"/>
+      <c r="AB87" s="27"/>
+      <c r="AC87" s="27"/>
+    </row>
+    <row r="88" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J88" s="27"/>
       <c r="K88" s="27"/>
       <c r="L88" s="27"/>
@@ -30716,10 +30763,10 @@
       <c r="Y88" s="27"/>
       <c r="Z88" s="27"/>
       <c r="AA88" s="27"/>
-    </row>
-    <row r="89" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
+      <c r="AB88" s="27"/>
+      <c r="AC88" s="27"/>
+    </row>
+    <row r="89" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J89" s="27"/>
       <c r="K89" s="27"/>
       <c r="L89" s="27"/>
@@ -30738,10 +30785,10 @@
       <c r="Y89" s="27"/>
       <c r="Z89" s="27"/>
       <c r="AA89" s="27"/>
-    </row>
-    <row r="90" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H90" s="27"/>
-      <c r="I90" s="27"/>
+      <c r="AB89" s="27"/>
+      <c r="AC89" s="27"/>
+    </row>
+    <row r="90" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J90" s="27"/>
       <c r="K90" s="27"/>
       <c r="L90" s="27"/>
@@ -30760,10 +30807,10 @@
       <c r="Y90" s="27"/>
       <c r="Z90" s="27"/>
       <c r="AA90" s="27"/>
-    </row>
-    <row r="91" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H91" s="27"/>
-      <c r="I91" s="27"/>
+      <c r="AB90" s="27"/>
+      <c r="AC90" s="27"/>
+    </row>
+    <row r="91" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J91" s="27"/>
       <c r="K91" s="27"/>
       <c r="L91" s="27"/>
@@ -30782,10 +30829,10 @@
       <c r="Y91" s="27"/>
       <c r="Z91" s="27"/>
       <c r="AA91" s="27"/>
-    </row>
-    <row r="92" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H92" s="27"/>
-      <c r="I92" s="27"/>
+      <c r="AB91" s="27"/>
+      <c r="AC91" s="27"/>
+    </row>
+    <row r="92" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J92" s="27"/>
       <c r="K92" s="27"/>
       <c r="L92" s="27"/>
@@ -30804,10 +30851,10 @@
       <c r="Y92" s="27"/>
       <c r="Z92" s="27"/>
       <c r="AA92" s="27"/>
-    </row>
-    <row r="93" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H93" s="27"/>
-      <c r="I93" s="27"/>
+      <c r="AB92" s="27"/>
+      <c r="AC92" s="27"/>
+    </row>
+    <row r="93" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J93" s="27"/>
       <c r="K93" s="27"/>
       <c r="L93" s="27"/>
@@ -30826,10 +30873,10 @@
       <c r="Y93" s="27"/>
       <c r="Z93" s="27"/>
       <c r="AA93" s="27"/>
-    </row>
-    <row r="94" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H94" s="27"/>
-      <c r="I94" s="27"/>
+      <c r="AB93" s="27"/>
+      <c r="AC93" s="27"/>
+    </row>
+    <row r="94" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J94" s="27"/>
       <c r="K94" s="27"/>
       <c r="L94" s="27"/>
@@ -30848,10 +30895,10 @@
       <c r="Y94" s="27"/>
       <c r="Z94" s="27"/>
       <c r="AA94" s="27"/>
-    </row>
-    <row r="95" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H95" s="27"/>
-      <c r="I95" s="27"/>
+      <c r="AB94" s="27"/>
+      <c r="AC94" s="27"/>
+    </row>
+    <row r="95" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J95" s="27"/>
       <c r="K95" s="27"/>
       <c r="L95" s="27"/>
@@ -30870,10 +30917,10 @@
       <c r="Y95" s="27"/>
       <c r="Z95" s="27"/>
       <c r="AA95" s="27"/>
-    </row>
-    <row r="96" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H96" s="27"/>
-      <c r="I96" s="27"/>
+      <c r="AB95" s="27"/>
+      <c r="AC95" s="27"/>
+    </row>
+    <row r="96" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J96" s="27"/>
       <c r="K96" s="27"/>
       <c r="L96" s="27"/>
@@ -30892,10 +30939,10 @@
       <c r="Y96" s="27"/>
       <c r="Z96" s="27"/>
       <c r="AA96" s="27"/>
-    </row>
-    <row r="97" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H97" s="27"/>
-      <c r="I97" s="27"/>
+      <c r="AB96" s="27"/>
+      <c r="AC96" s="27"/>
+    </row>
+    <row r="97" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J97" s="27"/>
       <c r="K97" s="27"/>
       <c r="L97" s="27"/>
@@ -30914,10 +30961,10 @@
       <c r="Y97" s="27"/>
       <c r="Z97" s="27"/>
       <c r="AA97" s="27"/>
-    </row>
-    <row r="98" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H98" s="27"/>
-      <c r="I98" s="27"/>
+      <c r="AB97" s="27"/>
+      <c r="AC97" s="27"/>
+    </row>
+    <row r="98" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J98" s="27"/>
       <c r="K98" s="27"/>
       <c r="L98" s="27"/>
@@ -30936,10 +30983,10 @@
       <c r="Y98" s="27"/>
       <c r="Z98" s="27"/>
       <c r="AA98" s="27"/>
-    </row>
-    <row r="99" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H99" s="27"/>
-      <c r="I99" s="27"/>
+      <c r="AB98" s="27"/>
+      <c r="AC98" s="27"/>
+    </row>
+    <row r="99" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J99" s="27"/>
       <c r="K99" s="27"/>
       <c r="L99" s="27"/>
@@ -30958,10 +31005,10 @@
       <c r="Y99" s="27"/>
       <c r="Z99" s="27"/>
       <c r="AA99" s="27"/>
-    </row>
-    <row r="100" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H100" s="27"/>
-      <c r="I100" s="27"/>
+      <c r="AB99" s="27"/>
+      <c r="AC99" s="27"/>
+    </row>
+    <row r="100" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J100" s="27"/>
       <c r="K100" s="27"/>
       <c r="L100" s="27"/>
@@ -30980,10 +31027,10 @@
       <c r="Y100" s="27"/>
       <c r="Z100" s="27"/>
       <c r="AA100" s="27"/>
-    </row>
-    <row r="101" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H101" s="27"/>
-      <c r="I101" s="27"/>
+      <c r="AB100" s="27"/>
+      <c r="AC100" s="27"/>
+    </row>
+    <row r="101" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J101" s="27"/>
       <c r="K101" s="27"/>
       <c r="L101" s="27"/>
@@ -31002,10 +31049,10 @@
       <c r="Y101" s="27"/>
       <c r="Z101" s="27"/>
       <c r="AA101" s="27"/>
-    </row>
-    <row r="102" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H102" s="27"/>
-      <c r="I102" s="27"/>
+      <c r="AB101" s="27"/>
+      <c r="AC101" s="27"/>
+    </row>
+    <row r="102" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J102" s="27"/>
       <c r="K102" s="27"/>
       <c r="L102" s="27"/>
@@ -31024,10 +31071,10 @@
       <c r="Y102" s="27"/>
       <c r="Z102" s="27"/>
       <c r="AA102" s="27"/>
-    </row>
-    <row r="103" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H103" s="27"/>
-      <c r="I103" s="27"/>
+      <c r="AB102" s="27"/>
+      <c r="AC102" s="27"/>
+    </row>
+    <row r="103" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J103" s="27"/>
       <c r="K103" s="27"/>
       <c r="L103" s="27"/>
@@ -31046,10 +31093,10 @@
       <c r="Y103" s="27"/>
       <c r="Z103" s="27"/>
       <c r="AA103" s="27"/>
-    </row>
-    <row r="104" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H104" s="27"/>
-      <c r="I104" s="27"/>
+      <c r="AB103" s="27"/>
+      <c r="AC103" s="27"/>
+    </row>
+    <row r="104" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J104" s="27"/>
       <c r="K104" s="27"/>
       <c r="L104" s="27"/>
@@ -31068,10 +31115,10 @@
       <c r="Y104" s="27"/>
       <c r="Z104" s="27"/>
       <c r="AA104" s="27"/>
-    </row>
-    <row r="105" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H105" s="27"/>
-      <c r="I105" s="27"/>
+      <c r="AB104" s="27"/>
+      <c r="AC104" s="27"/>
+    </row>
+    <row r="105" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J105" s="27"/>
       <c r="K105" s="27"/>
       <c r="L105" s="27"/>
@@ -31090,10 +31137,10 @@
       <c r="Y105" s="27"/>
       <c r="Z105" s="27"/>
       <c r="AA105" s="27"/>
-    </row>
-    <row r="106" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H106" s="27"/>
-      <c r="I106" s="27"/>
+      <c r="AB105" s="27"/>
+      <c r="AC105" s="27"/>
+    </row>
+    <row r="106" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J106" s="27"/>
       <c r="K106" s="27"/>
       <c r="L106" s="27"/>
@@ -31112,10 +31159,10 @@
       <c r="Y106" s="27"/>
       <c r="Z106" s="27"/>
       <c r="AA106" s="27"/>
-    </row>
-    <row r="107" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H107" s="27"/>
-      <c r="I107" s="27"/>
+      <c r="AB106" s="27"/>
+      <c r="AC106" s="27"/>
+    </row>
+    <row r="107" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J107" s="27"/>
       <c r="K107" s="27"/>
       <c r="L107" s="27"/>
@@ -31134,10 +31181,10 @@
       <c r="Y107" s="27"/>
       <c r="Z107" s="27"/>
       <c r="AA107" s="27"/>
-    </row>
-    <row r="108" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H108" s="27"/>
-      <c r="I108" s="27"/>
+      <c r="AB107" s="27"/>
+      <c r="AC107" s="27"/>
+    </row>
+    <row r="108" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J108" s="27"/>
       <c r="K108" s="27"/>
       <c r="L108" s="27"/>
@@ -31156,10 +31203,10 @@
       <c r="Y108" s="27"/>
       <c r="Z108" s="27"/>
       <c r="AA108" s="27"/>
-    </row>
-    <row r="109" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H109" s="27"/>
-      <c r="I109" s="27"/>
+      <c r="AB108" s="27"/>
+      <c r="AC108" s="27"/>
+    </row>
+    <row r="109" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J109" s="27"/>
       <c r="K109" s="27"/>
       <c r="L109" s="27"/>
@@ -31178,10 +31225,10 @@
       <c r="Y109" s="27"/>
       <c r="Z109" s="27"/>
       <c r="AA109" s="27"/>
-    </row>
-    <row r="110" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H110" s="27"/>
-      <c r="I110" s="27"/>
+      <c r="AB109" s="27"/>
+      <c r="AC109" s="27"/>
+    </row>
+    <row r="110" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J110" s="27"/>
       <c r="K110" s="27"/>
       <c r="L110" s="27"/>
@@ -31200,10 +31247,10 @@
       <c r="Y110" s="27"/>
       <c r="Z110" s="27"/>
       <c r="AA110" s="27"/>
-    </row>
-    <row r="111" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H111" s="27"/>
-      <c r="I111" s="27"/>
+      <c r="AB110" s="27"/>
+      <c r="AC110" s="27"/>
+    </row>
+    <row r="111" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J111" s="27"/>
       <c r="K111" s="27"/>
       <c r="L111" s="27"/>
@@ -31222,10 +31269,10 @@
       <c r="Y111" s="27"/>
       <c r="Z111" s="27"/>
       <c r="AA111" s="27"/>
-    </row>
-    <row r="112" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H112" s="27"/>
-      <c r="I112" s="27"/>
+      <c r="AB111" s="27"/>
+      <c r="AC111" s="27"/>
+    </row>
+    <row r="112" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J112" s="27"/>
       <c r="K112" s="27"/>
       <c r="L112" s="27"/>
@@ -31244,10 +31291,10 @@
       <c r="Y112" s="27"/>
       <c r="Z112" s="27"/>
       <c r="AA112" s="27"/>
-    </row>
-    <row r="113" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H113" s="27"/>
-      <c r="I113" s="27"/>
+      <c r="AB112" s="27"/>
+      <c r="AC112" s="27"/>
+    </row>
+    <row r="113" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J113" s="27"/>
       <c r="K113" s="27"/>
       <c r="L113" s="27"/>
@@ -31266,10 +31313,10 @@
       <c r="Y113" s="27"/>
       <c r="Z113" s="27"/>
       <c r="AA113" s="27"/>
-    </row>
-    <row r="114" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H114" s="27"/>
-      <c r="I114" s="27"/>
+      <c r="AB113" s="27"/>
+      <c r="AC113" s="27"/>
+    </row>
+    <row r="114" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J114" s="27"/>
       <c r="K114" s="27"/>
       <c r="L114" s="27"/>
@@ -31288,10 +31335,10 @@
       <c r="Y114" s="27"/>
       <c r="Z114" s="27"/>
       <c r="AA114" s="27"/>
-    </row>
-    <row r="115" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H115" s="27"/>
-      <c r="I115" s="27"/>
+      <c r="AB114" s="27"/>
+      <c r="AC114" s="27"/>
+    </row>
+    <row r="115" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J115" s="27"/>
       <c r="K115" s="27"/>
       <c r="L115" s="27"/>
@@ -31310,10 +31357,10 @@
       <c r="Y115" s="27"/>
       <c r="Z115" s="27"/>
       <c r="AA115" s="27"/>
-    </row>
-    <row r="116" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H116" s="27"/>
-      <c r="I116" s="27"/>
+      <c r="AB115" s="27"/>
+      <c r="AC115" s="27"/>
+    </row>
+    <row r="116" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J116" s="27"/>
       <c r="K116" s="27"/>
       <c r="L116" s="27"/>
@@ -31332,10 +31379,10 @@
       <c r="Y116" s="27"/>
       <c r="Z116" s="27"/>
       <c r="AA116" s="27"/>
-    </row>
-    <row r="117" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H117" s="27"/>
-      <c r="I117" s="27"/>
+      <c r="AB116" s="27"/>
+      <c r="AC116" s="27"/>
+    </row>
+    <row r="117" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J117" s="27"/>
       <c r="K117" s="27"/>
       <c r="L117" s="27"/>
@@ -31354,10 +31401,10 @@
       <c r="Y117" s="27"/>
       <c r="Z117" s="27"/>
       <c r="AA117" s="27"/>
-    </row>
-    <row r="118" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H118" s="27"/>
-      <c r="I118" s="27"/>
+      <c r="AB117" s="27"/>
+      <c r="AC117" s="27"/>
+    </row>
+    <row r="118" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J118" s="27"/>
       <c r="K118" s="27"/>
       <c r="L118" s="27"/>
@@ -31376,10 +31423,10 @@
       <c r="Y118" s="27"/>
       <c r="Z118" s="27"/>
       <c r="AA118" s="27"/>
-    </row>
-    <row r="119" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H119" s="27"/>
-      <c r="I119" s="27"/>
+      <c r="AB118" s="27"/>
+      <c r="AC118" s="27"/>
+    </row>
+    <row r="119" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J119" s="27"/>
       <c r="K119" s="27"/>
       <c r="L119" s="27"/>
@@ -31398,10 +31445,10 @@
       <c r="Y119" s="27"/>
       <c r="Z119" s="27"/>
       <c r="AA119" s="27"/>
-    </row>
-    <row r="120" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H120" s="27"/>
-      <c r="I120" s="27"/>
+      <c r="AB119" s="27"/>
+      <c r="AC119" s="27"/>
+    </row>
+    <row r="120" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J120" s="27"/>
       <c r="K120" s="27"/>
       <c r="L120" s="27"/>
@@ -31420,10 +31467,10 @@
       <c r="Y120" s="27"/>
       <c r="Z120" s="27"/>
       <c r="AA120" s="27"/>
-    </row>
-    <row r="121" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H121" s="27"/>
-      <c r="I121" s="27"/>
+      <c r="AB120" s="27"/>
+      <c r="AC120" s="27"/>
+    </row>
+    <row r="121" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J121" s="27"/>
       <c r="K121" s="27"/>
       <c r="L121" s="27"/>
@@ -31442,10 +31489,10 @@
       <c r="Y121" s="27"/>
       <c r="Z121" s="27"/>
       <c r="AA121" s="27"/>
-    </row>
-    <row r="122" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H122" s="27"/>
-      <c r="I122" s="27"/>
+      <c r="AB121" s="27"/>
+      <c r="AC121" s="27"/>
+    </row>
+    <row r="122" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J122" s="27"/>
       <c r="K122" s="27"/>
       <c r="L122" s="27"/>
@@ -31464,10 +31511,10 @@
       <c r="Y122" s="27"/>
       <c r="Z122" s="27"/>
       <c r="AA122" s="27"/>
-    </row>
-    <row r="123" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H123" s="27"/>
-      <c r="I123" s="27"/>
+      <c r="AB122" s="27"/>
+      <c r="AC122" s="27"/>
+    </row>
+    <row r="123" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J123" s="27"/>
       <c r="K123" s="27"/>
       <c r="L123" s="27"/>
@@ -31486,10 +31533,10 @@
       <c r="Y123" s="27"/>
       <c r="Z123" s="27"/>
       <c r="AA123" s="27"/>
-    </row>
-    <row r="124" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H124" s="27"/>
-      <c r="I124" s="27"/>
+      <c r="AB123" s="27"/>
+      <c r="AC123" s="27"/>
+    </row>
+    <row r="124" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J124" s="27"/>
       <c r="K124" s="27"/>
       <c r="L124" s="27"/>
@@ -31508,10 +31555,10 @@
       <c r="Y124" s="27"/>
       <c r="Z124" s="27"/>
       <c r="AA124" s="27"/>
-    </row>
-    <row r="125" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H125" s="27"/>
-      <c r="I125" s="27"/>
+      <c r="AB124" s="27"/>
+      <c r="AC124" s="27"/>
+    </row>
+    <row r="125" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J125" s="27"/>
       <c r="K125" s="27"/>
       <c r="L125" s="27"/>
@@ -31530,10 +31577,10 @@
       <c r="Y125" s="27"/>
       <c r="Z125" s="27"/>
       <c r="AA125" s="27"/>
-    </row>
-    <row r="126" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H126" s="27"/>
-      <c r="I126" s="27"/>
+      <c r="AB125" s="27"/>
+      <c r="AC125" s="27"/>
+    </row>
+    <row r="126" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J126" s="27"/>
       <c r="K126" s="27"/>
       <c r="L126" s="27"/>
@@ -31552,10 +31599,10 @@
       <c r="Y126" s="27"/>
       <c r="Z126" s="27"/>
       <c r="AA126" s="27"/>
-    </row>
-    <row r="127" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H127" s="27"/>
-      <c r="I127" s="27"/>
+      <c r="AB126" s="27"/>
+      <c r="AC126" s="27"/>
+    </row>
+    <row r="127" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J127" s="27"/>
       <c r="K127" s="27"/>
       <c r="L127" s="27"/>
@@ -31574,10 +31621,10 @@
       <c r="Y127" s="27"/>
       <c r="Z127" s="27"/>
       <c r="AA127" s="27"/>
-    </row>
-    <row r="128" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H128" s="27"/>
-      <c r="I128" s="27"/>
+      <c r="AB127" s="27"/>
+      <c r="AC127" s="27"/>
+    </row>
+    <row r="128" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J128" s="27"/>
       <c r="K128" s="27"/>
       <c r="L128" s="27"/>
@@ -31596,10 +31643,10 @@
       <c r="Y128" s="27"/>
       <c r="Z128" s="27"/>
       <c r="AA128" s="27"/>
-    </row>
-    <row r="129" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H129" s="27"/>
-      <c r="I129" s="27"/>
+      <c r="AB128" s="27"/>
+      <c r="AC128" s="27"/>
+    </row>
+    <row r="129" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J129" s="27"/>
       <c r="K129" s="27"/>
       <c r="L129" s="27"/>
@@ -31618,10 +31665,10 @@
       <c r="Y129" s="27"/>
       <c r="Z129" s="27"/>
       <c r="AA129" s="27"/>
-    </row>
-    <row r="130" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H130" s="27"/>
-      <c r="I130" s="27"/>
+      <c r="AB129" s="27"/>
+      <c r="AC129" s="27"/>
+    </row>
+    <row r="130" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J130" s="27"/>
       <c r="K130" s="27"/>
       <c r="L130" s="27"/>
@@ -31640,10 +31687,10 @@
       <c r="Y130" s="27"/>
       <c r="Z130" s="27"/>
       <c r="AA130" s="27"/>
-    </row>
-    <row r="131" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H131" s="27"/>
-      <c r="I131" s="27"/>
+      <c r="AB130" s="27"/>
+      <c r="AC130" s="27"/>
+    </row>
+    <row r="131" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J131" s="27"/>
       <c r="K131" s="27"/>
       <c r="L131" s="27"/>
@@ -31662,10 +31709,10 @@
       <c r="Y131" s="27"/>
       <c r="Z131" s="27"/>
       <c r="AA131" s="27"/>
-    </row>
-    <row r="132" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H132" s="27"/>
-      <c r="I132" s="27"/>
+      <c r="AB131" s="27"/>
+      <c r="AC131" s="27"/>
+    </row>
+    <row r="132" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J132" s="27"/>
       <c r="K132" s="27"/>
       <c r="L132" s="27"/>
@@ -31684,10 +31731,10 @@
       <c r="Y132" s="27"/>
       <c r="Z132" s="27"/>
       <c r="AA132" s="27"/>
-    </row>
-    <row r="133" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H133" s="27"/>
-      <c r="I133" s="27"/>
+      <c r="AB132" s="27"/>
+      <c r="AC132" s="27"/>
+    </row>
+    <row r="133" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J133" s="27"/>
       <c r="K133" s="27"/>
       <c r="L133" s="27"/>
@@ -31706,10 +31753,10 @@
       <c r="Y133" s="27"/>
       <c r="Z133" s="27"/>
       <c r="AA133" s="27"/>
-    </row>
-    <row r="134" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H134" s="27"/>
-      <c r="I134" s="27"/>
+      <c r="AB133" s="27"/>
+      <c r="AC133" s="27"/>
+    </row>
+    <row r="134" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J134" s="27"/>
       <c r="K134" s="27"/>
       <c r="L134" s="27"/>
@@ -31728,10 +31775,10 @@
       <c r="Y134" s="27"/>
       <c r="Z134" s="27"/>
       <c r="AA134" s="27"/>
-    </row>
-    <row r="135" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H135" s="27"/>
-      <c r="I135" s="27"/>
+      <c r="AB134" s="27"/>
+      <c r="AC134" s="27"/>
+    </row>
+    <row r="135" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J135" s="27"/>
       <c r="K135" s="27"/>
       <c r="L135" s="27"/>
@@ -31750,10 +31797,10 @@
       <c r="Y135" s="27"/>
       <c r="Z135" s="27"/>
       <c r="AA135" s="27"/>
-    </row>
-    <row r="136" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H136" s="27"/>
-      <c r="I136" s="27"/>
+      <c r="AB135" s="27"/>
+      <c r="AC135" s="27"/>
+    </row>
+    <row r="136" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J136" s="27"/>
       <c r="K136" s="27"/>
       <c r="L136" s="27"/>
@@ -31772,10 +31819,10 @@
       <c r="Y136" s="27"/>
       <c r="Z136" s="27"/>
       <c r="AA136" s="27"/>
-    </row>
-    <row r="137" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H137" s="27"/>
-      <c r="I137" s="27"/>
+      <c r="AB136" s="27"/>
+      <c r="AC136" s="27"/>
+    </row>
+    <row r="137" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J137" s="27"/>
       <c r="K137" s="27"/>
       <c r="L137" s="27"/>
@@ -31794,10 +31841,10 @@
       <c r="Y137" s="27"/>
       <c r="Z137" s="27"/>
       <c r="AA137" s="27"/>
-    </row>
-    <row r="138" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H138" s="27"/>
-      <c r="I138" s="27"/>
+      <c r="AB137" s="27"/>
+      <c r="AC137" s="27"/>
+    </row>
+    <row r="138" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J138" s="27"/>
       <c r="K138" s="27"/>
       <c r="L138" s="27"/>
@@ -31816,10 +31863,10 @@
       <c r="Y138" s="27"/>
       <c r="Z138" s="27"/>
       <c r="AA138" s="27"/>
-    </row>
-    <row r="139" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H139" s="27"/>
-      <c r="I139" s="27"/>
+      <c r="AB138" s="27"/>
+      <c r="AC138" s="27"/>
+    </row>
+    <row r="139" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J139" s="27"/>
       <c r="K139" s="27"/>
       <c r="L139" s="27"/>
@@ -31838,10 +31885,10 @@
       <c r="Y139" s="27"/>
       <c r="Z139" s="27"/>
       <c r="AA139" s="27"/>
-    </row>
-    <row r="140" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H140" s="27"/>
-      <c r="I140" s="27"/>
+      <c r="AB139" s="27"/>
+      <c r="AC139" s="27"/>
+    </row>
+    <row r="140" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J140" s="27"/>
       <c r="K140" s="27"/>
       <c r="L140" s="27"/>
@@ -31860,10 +31907,10 @@
       <c r="Y140" s="27"/>
       <c r="Z140" s="27"/>
       <c r="AA140" s="27"/>
-    </row>
-    <row r="141" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H141" s="27"/>
-      <c r="I141" s="27"/>
+      <c r="AB140" s="27"/>
+      <c r="AC140" s="27"/>
+    </row>
+    <row r="141" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J141" s="27"/>
       <c r="K141" s="27"/>
       <c r="L141" s="27"/>
@@ -31882,10 +31929,10 @@
       <c r="Y141" s="27"/>
       <c r="Z141" s="27"/>
       <c r="AA141" s="27"/>
-    </row>
-    <row r="142" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H142" s="27"/>
-      <c r="I142" s="27"/>
+      <c r="AB141" s="27"/>
+      <c r="AC141" s="27"/>
+    </row>
+    <row r="142" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J142" s="27"/>
       <c r="K142" s="27"/>
       <c r="L142" s="27"/>
@@ -31904,10 +31951,10 @@
       <c r="Y142" s="27"/>
       <c r="Z142" s="27"/>
       <c r="AA142" s="27"/>
-    </row>
-    <row r="143" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H143" s="27"/>
-      <c r="I143" s="27"/>
+      <c r="AB142" s="27"/>
+      <c r="AC142" s="27"/>
+    </row>
+    <row r="143" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J143" s="27"/>
       <c r="K143" s="27"/>
       <c r="L143" s="27"/>
@@ -31926,10 +31973,10 @@
       <c r="Y143" s="27"/>
       <c r="Z143" s="27"/>
       <c r="AA143" s="27"/>
-    </row>
-    <row r="144" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H144" s="27"/>
-      <c r="I144" s="27"/>
+      <c r="AB143" s="27"/>
+      <c r="AC143" s="27"/>
+    </row>
+    <row r="144" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J144" s="27"/>
       <c r="K144" s="27"/>
       <c r="L144" s="27"/>
@@ -31948,10 +31995,10 @@
       <c r="Y144" s="27"/>
       <c r="Z144" s="27"/>
       <c r="AA144" s="27"/>
-    </row>
-    <row r="145" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H145" s="27"/>
-      <c r="I145" s="27"/>
+      <c r="AB144" s="27"/>
+      <c r="AC144" s="27"/>
+    </row>
+    <row r="145" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J145" s="27"/>
       <c r="K145" s="27"/>
       <c r="L145" s="27"/>
@@ -31970,10 +32017,10 @@
       <c r="Y145" s="27"/>
       <c r="Z145" s="27"/>
       <c r="AA145" s="27"/>
-    </row>
-    <row r="146" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H146" s="27"/>
-      <c r="I146" s="27"/>
+      <c r="AB145" s="27"/>
+      <c r="AC145" s="27"/>
+    </row>
+    <row r="146" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J146" s="27"/>
       <c r="K146" s="27"/>
       <c r="L146" s="27"/>
@@ -31992,10 +32039,10 @@
       <c r="Y146" s="27"/>
       <c r="Z146" s="27"/>
       <c r="AA146" s="27"/>
-    </row>
-    <row r="147" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H147" s="27"/>
-      <c r="I147" s="27"/>
+      <c r="AB146" s="27"/>
+      <c r="AC146" s="27"/>
+    </row>
+    <row r="147" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J147" s="27"/>
       <c r="K147" s="27"/>
       <c r="L147" s="27"/>
@@ -32014,10 +32061,10 @@
       <c r="Y147" s="27"/>
       <c r="Z147" s="27"/>
       <c r="AA147" s="27"/>
-    </row>
-    <row r="148" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H148" s="27"/>
-      <c r="I148" s="27"/>
+      <c r="AB147" s="27"/>
+      <c r="AC147" s="27"/>
+    </row>
+    <row r="148" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J148" s="27"/>
       <c r="K148" s="27"/>
       <c r="L148" s="27"/>
@@ -32036,10 +32083,10 @@
       <c r="Y148" s="27"/>
       <c r="Z148" s="27"/>
       <c r="AA148" s="27"/>
-    </row>
-    <row r="149" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H149" s="27"/>
-      <c r="I149" s="27"/>
+      <c r="AB148" s="27"/>
+      <c r="AC148" s="27"/>
+    </row>
+    <row r="149" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J149" s="27"/>
       <c r="K149" s="27"/>
       <c r="L149" s="27"/>
@@ -32058,10 +32105,10 @@
       <c r="Y149" s="27"/>
       <c r="Z149" s="27"/>
       <c r="AA149" s="27"/>
-    </row>
-    <row r="150" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H150" s="27"/>
-      <c r="I150" s="27"/>
+      <c r="AB149" s="27"/>
+      <c r="AC149" s="27"/>
+    </row>
+    <row r="150" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J150" s="27"/>
       <c r="K150" s="27"/>
       <c r="L150" s="27"/>
@@ -32080,10 +32127,10 @@
       <c r="Y150" s="27"/>
       <c r="Z150" s="27"/>
       <c r="AA150" s="27"/>
-    </row>
-    <row r="151" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H151" s="27"/>
-      <c r="I151" s="27"/>
+      <c r="AB150" s="27"/>
+      <c r="AC150" s="27"/>
+    </row>
+    <row r="151" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J151" s="27"/>
       <c r="K151" s="27"/>
       <c r="L151" s="27"/>
@@ -32102,10 +32149,10 @@
       <c r="Y151" s="27"/>
       <c r="Z151" s="27"/>
       <c r="AA151" s="27"/>
-    </row>
-    <row r="152" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H152" s="27"/>
-      <c r="I152" s="27"/>
+      <c r="AB151" s="27"/>
+      <c r="AC151" s="27"/>
+    </row>
+    <row r="152" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J152" s="27"/>
       <c r="K152" s="27"/>
       <c r="L152" s="27"/>
@@ -32124,10 +32171,10 @@
       <c r="Y152" s="27"/>
       <c r="Z152" s="27"/>
       <c r="AA152" s="27"/>
-    </row>
-    <row r="153" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H153" s="27"/>
-      <c r="I153" s="27"/>
+      <c r="AB152" s="27"/>
+      <c r="AC152" s="27"/>
+    </row>
+    <row r="153" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J153" s="27"/>
       <c r="K153" s="27"/>
       <c r="L153" s="27"/>
@@ -32146,10 +32193,10 @@
       <c r="Y153" s="27"/>
       <c r="Z153" s="27"/>
       <c r="AA153" s="27"/>
-    </row>
-    <row r="154" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H154" s="27"/>
-      <c r="I154" s="27"/>
+      <c r="AB153" s="27"/>
+      <c r="AC153" s="27"/>
+    </row>
+    <row r="154" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J154" s="27"/>
       <c r="K154" s="27"/>
       <c r="L154" s="27"/>
@@ -32168,10 +32215,10 @@
       <c r="Y154" s="27"/>
       <c r="Z154" s="27"/>
       <c r="AA154" s="27"/>
-    </row>
-    <row r="155" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H155" s="27"/>
-      <c r="I155" s="27"/>
+      <c r="AB154" s="27"/>
+      <c r="AC154" s="27"/>
+    </row>
+    <row r="155" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J155" s="27"/>
       <c r="K155" s="27"/>
       <c r="L155" s="27"/>
@@ -32190,10 +32237,10 @@
       <c r="Y155" s="27"/>
       <c r="Z155" s="27"/>
       <c r="AA155" s="27"/>
-    </row>
-    <row r="156" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H156" s="27"/>
-      <c r="I156" s="27"/>
+      <c r="AB155" s="27"/>
+      <c r="AC155" s="27"/>
+    </row>
+    <row r="156" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J156" s="27"/>
       <c r="K156" s="27"/>
       <c r="L156" s="27"/>
@@ -32212,10 +32259,10 @@
       <c r="Y156" s="27"/>
       <c r="Z156" s="27"/>
       <c r="AA156" s="27"/>
-    </row>
-    <row r="157" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H157" s="27"/>
-      <c r="I157" s="27"/>
+      <c r="AB156" s="27"/>
+      <c r="AC156" s="27"/>
+    </row>
+    <row r="157" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J157" s="27"/>
       <c r="K157" s="27"/>
       <c r="L157" s="27"/>
@@ -32234,10 +32281,10 @@
       <c r="Y157" s="27"/>
       <c r="Z157" s="27"/>
       <c r="AA157" s="27"/>
-    </row>
-    <row r="158" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H158" s="27"/>
-      <c r="I158" s="27"/>
+      <c r="AB157" s="27"/>
+      <c r="AC157" s="27"/>
+    </row>
+    <row r="158" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J158" s="27"/>
       <c r="K158" s="27"/>
       <c r="L158" s="27"/>
@@ -32256,10 +32303,10 @@
       <c r="Y158" s="27"/>
       <c r="Z158" s="27"/>
       <c r="AA158" s="27"/>
-    </row>
-    <row r="159" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H159" s="27"/>
-      <c r="I159" s="27"/>
+      <c r="AB158" s="27"/>
+      <c r="AC158" s="27"/>
+    </row>
+    <row r="159" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J159" s="27"/>
       <c r="K159" s="27"/>
       <c r="L159" s="27"/>
@@ -32278,10 +32325,10 @@
       <c r="Y159" s="27"/>
       <c r="Z159" s="27"/>
       <c r="AA159" s="27"/>
-    </row>
-    <row r="160" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H160" s="27"/>
-      <c r="I160" s="27"/>
+      <c r="AB159" s="27"/>
+      <c r="AC159" s="27"/>
+    </row>
+    <row r="160" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J160" s="27"/>
       <c r="K160" s="27"/>
       <c r="L160" s="27"/>
@@ -32300,10 +32347,10 @@
       <c r="Y160" s="27"/>
       <c r="Z160" s="27"/>
       <c r="AA160" s="27"/>
-    </row>
-    <row r="161" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H161" s="27"/>
-      <c r="I161" s="27"/>
+      <c r="AB160" s="27"/>
+      <c r="AC160" s="27"/>
+    </row>
+    <row r="161" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J161" s="27"/>
       <c r="K161" s="27"/>
       <c r="L161" s="27"/>
@@ -32322,10 +32369,10 @@
       <c r="Y161" s="27"/>
       <c r="Z161" s="27"/>
       <c r="AA161" s="27"/>
-    </row>
-    <row r="162" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H162" s="27"/>
-      <c r="I162" s="27"/>
+      <c r="AB161" s="27"/>
+      <c r="AC161" s="27"/>
+    </row>
+    <row r="162" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J162" s="27"/>
       <c r="K162" s="27"/>
       <c r="L162" s="27"/>
@@ -32344,10 +32391,10 @@
       <c r="Y162" s="27"/>
       <c r="Z162" s="27"/>
       <c r="AA162" s="27"/>
-    </row>
-    <row r="163" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H163" s="27"/>
-      <c r="I163" s="27"/>
+      <c r="AB162" s="27"/>
+      <c r="AC162" s="27"/>
+    </row>
+    <row r="163" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J163" s="27"/>
       <c r="K163" s="27"/>
       <c r="L163" s="27"/>
@@ -32366,10 +32413,10 @@
       <c r="Y163" s="27"/>
       <c r="Z163" s="27"/>
       <c r="AA163" s="27"/>
-    </row>
-    <row r="164" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H164" s="27"/>
-      <c r="I164" s="27"/>
+      <c r="AB163" s="27"/>
+      <c r="AC163" s="27"/>
+    </row>
+    <row r="164" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J164" s="27"/>
       <c r="K164" s="27"/>
       <c r="L164" s="27"/>
@@ -32388,10 +32435,10 @@
       <c r="Y164" s="27"/>
       <c r="Z164" s="27"/>
       <c r="AA164" s="27"/>
-    </row>
-    <row r="165" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H165" s="27"/>
-      <c r="I165" s="27"/>
+      <c r="AB164" s="27"/>
+      <c r="AC164" s="27"/>
+    </row>
+    <row r="165" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J165" s="27"/>
       <c r="K165" s="27"/>
       <c r="L165" s="27"/>
@@ -32410,10 +32457,10 @@
       <c r="Y165" s="27"/>
       <c r="Z165" s="27"/>
       <c r="AA165" s="27"/>
-    </row>
-    <row r="166" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H166" s="27"/>
-      <c r="I166" s="27"/>
+      <c r="AB165" s="27"/>
+      <c r="AC165" s="27"/>
+    </row>
+    <row r="166" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J166" s="27"/>
       <c r="K166" s="27"/>
       <c r="L166" s="27"/>
@@ -32432,10 +32479,10 @@
       <c r="Y166" s="27"/>
       <c r="Z166" s="27"/>
       <c r="AA166" s="27"/>
-    </row>
-    <row r="167" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H167" s="27"/>
-      <c r="I167" s="27"/>
+      <c r="AB166" s="27"/>
+      <c r="AC166" s="27"/>
+    </row>
+    <row r="167" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J167" s="27"/>
       <c r="K167" s="27"/>
       <c r="L167" s="27"/>
@@ -32454,10 +32501,10 @@
       <c r="Y167" s="27"/>
       <c r="Z167" s="27"/>
       <c r="AA167" s="27"/>
-    </row>
-    <row r="168" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H168" s="27"/>
-      <c r="I168" s="27"/>
+      <c r="AB167" s="27"/>
+      <c r="AC167" s="27"/>
+    </row>
+    <row r="168" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J168" s="27"/>
       <c r="K168" s="27"/>
       <c r="L168" s="27"/>
@@ -32476,10 +32523,10 @@
       <c r="Y168" s="27"/>
       <c r="Z168" s="27"/>
       <c r="AA168" s="27"/>
-    </row>
-    <row r="169" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H169" s="27"/>
-      <c r="I169" s="27"/>
+      <c r="AB168" s="27"/>
+      <c r="AC168" s="27"/>
+    </row>
+    <row r="169" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J169" s="27"/>
       <c r="K169" s="27"/>
       <c r="L169" s="27"/>
@@ -32498,10 +32545,10 @@
       <c r="Y169" s="27"/>
       <c r="Z169" s="27"/>
       <c r="AA169" s="27"/>
-    </row>
-    <row r="170" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H170" s="27"/>
-      <c r="I170" s="27"/>
+      <c r="AB169" s="27"/>
+      <c r="AC169" s="27"/>
+    </row>
+    <row r="170" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J170" s="27"/>
       <c r="K170" s="27"/>
       <c r="L170" s="27"/>
@@ -32520,10 +32567,10 @@
       <c r="Y170" s="27"/>
       <c r="Z170" s="27"/>
       <c r="AA170" s="27"/>
-    </row>
-    <row r="171" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H171" s="27"/>
-      <c r="I171" s="27"/>
+      <c r="AB170" s="27"/>
+      <c r="AC170" s="27"/>
+    </row>
+    <row r="171" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J171" s="27"/>
       <c r="K171" s="27"/>
       <c r="L171" s="27"/>
@@ -32542,10 +32589,10 @@
       <c r="Y171" s="27"/>
       <c r="Z171" s="27"/>
       <c r="AA171" s="27"/>
-    </row>
-    <row r="172" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H172" s="27"/>
-      <c r="I172" s="27"/>
+      <c r="AB171" s="27"/>
+      <c r="AC171" s="27"/>
+    </row>
+    <row r="172" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J172" s="27"/>
       <c r="K172" s="27"/>
       <c r="L172" s="27"/>
@@ -32564,10 +32611,10 @@
       <c r="Y172" s="27"/>
       <c r="Z172" s="27"/>
       <c r="AA172" s="27"/>
-    </row>
-    <row r="173" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H173" s="27"/>
-      <c r="I173" s="27"/>
+      <c r="AB172" s="27"/>
+      <c r="AC172" s="27"/>
+    </row>
+    <row r="173" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J173" s="27"/>
       <c r="K173" s="27"/>
       <c r="L173" s="27"/>
@@ -32586,10 +32633,10 @@
       <c r="Y173" s="27"/>
       <c r="Z173" s="27"/>
       <c r="AA173" s="27"/>
-    </row>
-    <row r="174" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H174" s="27"/>
-      <c r="I174" s="27"/>
+      <c r="AB173" s="27"/>
+      <c r="AC173" s="27"/>
+    </row>
+    <row r="174" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J174" s="27"/>
       <c r="K174" s="27"/>
       <c r="L174" s="27"/>
@@ -32608,10 +32655,10 @@
       <c r="Y174" s="27"/>
       <c r="Z174" s="27"/>
       <c r="AA174" s="27"/>
-    </row>
-    <row r="175" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H175" s="27"/>
-      <c r="I175" s="27"/>
+      <c r="AB174" s="27"/>
+      <c r="AC174" s="27"/>
+    </row>
+    <row r="175" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J175" s="27"/>
       <c r="K175" s="27"/>
       <c r="L175" s="27"/>
@@ -32630,10 +32677,10 @@
       <c r="Y175" s="27"/>
       <c r="Z175" s="27"/>
       <c r="AA175" s="27"/>
-    </row>
-    <row r="176" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H176" s="27"/>
-      <c r="I176" s="27"/>
+      <c r="AB175" s="27"/>
+      <c r="AC175" s="27"/>
+    </row>
+    <row r="176" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J176" s="27"/>
       <c r="K176" s="27"/>
       <c r="L176" s="27"/>
@@ -32652,10 +32699,10 @@
       <c r="Y176" s="27"/>
       <c r="Z176" s="27"/>
       <c r="AA176" s="27"/>
-    </row>
-    <row r="177" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="H177" s="27"/>
-      <c r="I177" s="27"/>
+      <c r="AB176" s="27"/>
+      <c r="AC176" s="27"/>
+    </row>
+    <row r="177" spans="5:29" x14ac:dyDescent="0.25">
       <c r="J177" s="27"/>
       <c r="K177" s="27"/>
       <c r="L177" s="27"/>
@@ -32674,10 +32721,10 @@
       <c r="Y177" s="27"/>
       <c r="Z177" s="27"/>
       <c r="AA177" s="27"/>
-    </row>
-    <row r="178" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="H178" s="27"/>
-      <c r="I178" s="27"/>
+      <c r="AB177" s="27"/>
+      <c r="AC177" s="27"/>
+    </row>
+    <row r="178" spans="5:29" x14ac:dyDescent="0.25">
       <c r="J178" s="27"/>
       <c r="K178" s="27"/>
       <c r="L178" s="27"/>
@@ -32696,10 +32743,10 @@
       <c r="Y178" s="27"/>
       <c r="Z178" s="27"/>
       <c r="AA178" s="27"/>
-    </row>
-    <row r="179" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="H179" s="27"/>
-      <c r="I179" s="27"/>
+      <c r="AB178" s="27"/>
+      <c r="AC178" s="27"/>
+    </row>
+    <row r="179" spans="5:29" x14ac:dyDescent="0.25">
       <c r="J179" s="27"/>
       <c r="K179" s="27"/>
       <c r="L179" s="27"/>
@@ -32718,10 +32765,10 @@
       <c r="Y179" s="27"/>
       <c r="Z179" s="27"/>
       <c r="AA179" s="27"/>
-    </row>
-    <row r="180" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="H180" s="27"/>
-      <c r="I180" s="27"/>
+      <c r="AB179" s="27"/>
+      <c r="AC179" s="27"/>
+    </row>
+    <row r="180" spans="5:29" x14ac:dyDescent="0.25">
       <c r="J180" s="27"/>
       <c r="K180" s="27"/>
       <c r="L180" s="27"/>
@@ -32740,10 +32787,10 @@
       <c r="Y180" s="27"/>
       <c r="Z180" s="27"/>
       <c r="AA180" s="27"/>
-    </row>
-    <row r="181" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="H181" s="27"/>
-      <c r="I181" s="27"/>
+      <c r="AB180" s="27"/>
+      <c r="AC180" s="27"/>
+    </row>
+    <row r="181" spans="5:29" x14ac:dyDescent="0.25">
       <c r="J181" s="27"/>
       <c r="K181" s="27"/>
       <c r="L181" s="27"/>
@@ -32762,10 +32809,10 @@
       <c r="Y181" s="27"/>
       <c r="Z181" s="27"/>
       <c r="AA181" s="27"/>
-    </row>
-    <row r="182" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="H182" s="27"/>
-      <c r="I182" s="27"/>
+      <c r="AB181" s="27"/>
+      <c r="AC181" s="27"/>
+    </row>
+    <row r="182" spans="5:29" x14ac:dyDescent="0.25">
       <c r="J182" s="27"/>
       <c r="K182" s="27"/>
       <c r="L182" s="27"/>
@@ -32784,10 +32831,10 @@
       <c r="Y182" s="27"/>
       <c r="Z182" s="27"/>
       <c r="AA182" s="27"/>
-    </row>
-    <row r="183" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="H183" s="27"/>
-      <c r="I183" s="27"/>
+      <c r="AB182" s="27"/>
+      <c r="AC182" s="27"/>
+    </row>
+    <row r="183" spans="5:29" x14ac:dyDescent="0.25">
       <c r="J183" s="27"/>
       <c r="K183" s="27"/>
       <c r="L183" s="27"/>
@@ -32806,15 +32853,15 @@
       <c r="Y183" s="27"/>
       <c r="Z183" s="27"/>
       <c r="AA183" s="27"/>
-    </row>
-    <row r="184" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C184" s="29"/>
-      <c r="D184" s="29"/>
+      <c r="AB183" s="27"/>
+      <c r="AC183" s="27"/>
+    </row>
+    <row r="184" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E184" s="29"/>
-      <c r="F184" s="30"/>
-      <c r="G184" s="31"/>
-      <c r="H184" s="27"/>
-      <c r="I184" s="27"/>
+      <c r="F184" s="29"/>
+      <c r="G184" s="29"/>
+      <c r="H184" s="30"/>
+      <c r="I184" s="31"/>
       <c r="J184" s="27"/>
       <c r="K184" s="27"/>
       <c r="L184" s="27"/>
@@ -32833,15 +32880,15 @@
       <c r="Y184" s="27"/>
       <c r="Z184" s="27"/>
       <c r="AA184" s="27"/>
-    </row>
-    <row r="185" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C185" s="29"/>
-      <c r="D185" s="29"/>
+      <c r="AB184" s="27"/>
+      <c r="AC184" s="27"/>
+    </row>
+    <row r="185" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E185" s="29"/>
-      <c r="F185" s="30"/>
-      <c r="G185" s="31"/>
-      <c r="H185" s="27"/>
-      <c r="I185" s="27"/>
+      <c r="F185" s="29"/>
+      <c r="G185" s="29"/>
+      <c r="H185" s="30"/>
+      <c r="I185" s="31"/>
       <c r="J185" s="27"/>
       <c r="K185" s="27"/>
       <c r="L185" s="27"/>
@@ -32860,15 +32907,15 @@
       <c r="Y185" s="27"/>
       <c r="Z185" s="27"/>
       <c r="AA185" s="27"/>
-    </row>
-    <row r="186" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C186" s="29"/>
-      <c r="D186" s="29"/>
+      <c r="AB185" s="27"/>
+      <c r="AC185" s="27"/>
+    </row>
+    <row r="186" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E186" s="29"/>
-      <c r="F186" s="30"/>
-      <c r="G186" s="31"/>
-      <c r="H186" s="27"/>
-      <c r="I186" s="27"/>
+      <c r="F186" s="29"/>
+      <c r="G186" s="29"/>
+      <c r="H186" s="30"/>
+      <c r="I186" s="31"/>
       <c r="J186" s="27"/>
       <c r="K186" s="27"/>
       <c r="L186" s="27"/>
@@ -32887,15 +32934,15 @@
       <c r="Y186" s="27"/>
       <c r="Z186" s="27"/>
       <c r="AA186" s="27"/>
-    </row>
-    <row r="187" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C187" s="29"/>
-      <c r="D187" s="29"/>
+      <c r="AB186" s="27"/>
+      <c r="AC186" s="27"/>
+    </row>
+    <row r="187" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E187" s="29"/>
-      <c r="F187" s="30"/>
-      <c r="G187" s="31"/>
-      <c r="H187" s="27"/>
-      <c r="I187" s="27"/>
+      <c r="F187" s="29"/>
+      <c r="G187" s="29"/>
+      <c r="H187" s="30"/>
+      <c r="I187" s="31"/>
       <c r="J187" s="27"/>
       <c r="K187" s="27"/>
       <c r="L187" s="27"/>
@@ -32914,15 +32961,15 @@
       <c r="Y187" s="27"/>
       <c r="Z187" s="27"/>
       <c r="AA187" s="27"/>
-    </row>
-    <row r="188" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C188" s="29"/>
-      <c r="D188" s="29"/>
+      <c r="AB187" s="27"/>
+      <c r="AC187" s="27"/>
+    </row>
+    <row r="188" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E188" s="29"/>
-      <c r="F188" s="30"/>
-      <c r="G188" s="31"/>
-      <c r="H188" s="27"/>
-      <c r="I188" s="27"/>
+      <c r="F188" s="29"/>
+      <c r="G188" s="29"/>
+      <c r="H188" s="30"/>
+      <c r="I188" s="31"/>
       <c r="J188" s="27"/>
       <c r="K188" s="27"/>
       <c r="L188" s="27"/>
@@ -32941,15 +32988,15 @@
       <c r="Y188" s="27"/>
       <c r="Z188" s="27"/>
       <c r="AA188" s="27"/>
-    </row>
-    <row r="189" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C189" s="29"/>
-      <c r="D189" s="29"/>
+      <c r="AB188" s="27"/>
+      <c r="AC188" s="27"/>
+    </row>
+    <row r="189" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E189" s="29"/>
-      <c r="F189" s="30"/>
-      <c r="G189" s="31"/>
-      <c r="H189" s="27"/>
-      <c r="I189" s="27"/>
+      <c r="F189" s="29"/>
+      <c r="G189" s="29"/>
+      <c r="H189" s="30"/>
+      <c r="I189" s="31"/>
       <c r="J189" s="27"/>
       <c r="K189" s="27"/>
       <c r="L189" s="27"/>
@@ -32968,15 +33015,15 @@
       <c r="Y189" s="27"/>
       <c r="Z189" s="27"/>
       <c r="AA189" s="27"/>
-    </row>
-    <row r="190" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C190" s="29"/>
-      <c r="D190" s="29"/>
+      <c r="AB189" s="27"/>
+      <c r="AC189" s="27"/>
+    </row>
+    <row r="190" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E190" s="29"/>
-      <c r="F190" s="30"/>
-      <c r="G190" s="31"/>
-      <c r="H190" s="27"/>
-      <c r="I190" s="27"/>
+      <c r="F190" s="29"/>
+      <c r="G190" s="29"/>
+      <c r="H190" s="30"/>
+      <c r="I190" s="31"/>
       <c r="J190" s="27"/>
       <c r="K190" s="27"/>
       <c r="L190" s="27"/>
@@ -32995,15 +33042,15 @@
       <c r="Y190" s="27"/>
       <c r="Z190" s="27"/>
       <c r="AA190" s="27"/>
-    </row>
-    <row r="191" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C191" s="31"/>
-      <c r="D191" s="31"/>
+      <c r="AB190" s="27"/>
+      <c r="AC190" s="27"/>
+    </row>
+    <row r="191" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E191" s="31"/>
-      <c r="F191" s="30"/>
+      <c r="F191" s="31"/>
       <c r="G191" s="31"/>
-      <c r="H191" s="27"/>
-      <c r="I191" s="27"/>
+      <c r="H191" s="30"/>
+      <c r="I191" s="31"/>
       <c r="J191" s="27"/>
       <c r="K191" s="27"/>
       <c r="L191" s="27"/>
@@ -33022,15 +33069,15 @@
       <c r="Y191" s="27"/>
       <c r="Z191" s="27"/>
       <c r="AA191" s="27"/>
-    </row>
-    <row r="192" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C192" s="31"/>
-      <c r="D192" s="31"/>
+      <c r="AB191" s="27"/>
+      <c r="AC191" s="27"/>
+    </row>
+    <row r="192" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E192" s="31"/>
-      <c r="F192" s="30"/>
+      <c r="F192" s="31"/>
       <c r="G192" s="31"/>
-      <c r="H192" s="27"/>
-      <c r="I192" s="27"/>
+      <c r="H192" s="30"/>
+      <c r="I192" s="31"/>
       <c r="J192" s="27"/>
       <c r="K192" s="27"/>
       <c r="L192" s="27"/>
@@ -33049,15 +33096,15 @@
       <c r="Y192" s="27"/>
       <c r="Z192" s="27"/>
       <c r="AA192" s="27"/>
-    </row>
-    <row r="193" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C193" s="31"/>
-      <c r="D193" s="31"/>
+      <c r="AB192" s="27"/>
+      <c r="AC192" s="27"/>
+    </row>
+    <row r="193" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E193" s="31"/>
-      <c r="F193" s="30"/>
+      <c r="F193" s="31"/>
       <c r="G193" s="31"/>
-      <c r="H193" s="27"/>
-      <c r="I193" s="27"/>
+      <c r="H193" s="30"/>
+      <c r="I193" s="31"/>
       <c r="J193" s="27"/>
       <c r="K193" s="27"/>
       <c r="L193" s="27"/>
@@ -33076,15 +33123,15 @@
       <c r="Y193" s="27"/>
       <c r="Z193" s="27"/>
       <c r="AA193" s="27"/>
-    </row>
-    <row r="194" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C194" s="31"/>
-      <c r="D194" s="31"/>
+      <c r="AB193" s="27"/>
+      <c r="AC193" s="27"/>
+    </row>
+    <row r="194" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E194" s="31"/>
-      <c r="F194" s="30"/>
+      <c r="F194" s="31"/>
       <c r="G194" s="31"/>
-      <c r="H194" s="27"/>
-      <c r="I194" s="27"/>
+      <c r="H194" s="30"/>
+      <c r="I194" s="31"/>
       <c r="J194" s="27"/>
       <c r="K194" s="27"/>
       <c r="L194" s="27"/>
@@ -33103,15 +33150,15 @@
       <c r="Y194" s="27"/>
       <c r="Z194" s="27"/>
       <c r="AA194" s="27"/>
-    </row>
-    <row r="195" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C195" s="31"/>
-      <c r="D195" s="31"/>
+      <c r="AB194" s="27"/>
+      <c r="AC194" s="27"/>
+    </row>
+    <row r="195" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E195" s="31"/>
-      <c r="F195" s="30"/>
+      <c r="F195" s="31"/>
       <c r="G195" s="31"/>
-      <c r="H195" s="27"/>
-      <c r="I195" s="27"/>
+      <c r="H195" s="30"/>
+      <c r="I195" s="31"/>
       <c r="J195" s="27"/>
       <c r="K195" s="27"/>
       <c r="L195" s="27"/>
@@ -33130,15 +33177,15 @@
       <c r="Y195" s="27"/>
       <c r="Z195" s="27"/>
       <c r="AA195" s="27"/>
-    </row>
-    <row r="196" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C196" s="31"/>
-      <c r="D196" s="31"/>
+      <c r="AB195" s="27"/>
+      <c r="AC195" s="27"/>
+    </row>
+    <row r="196" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E196" s="31"/>
-      <c r="F196" s="30"/>
+      <c r="F196" s="31"/>
       <c r="G196" s="31"/>
-      <c r="H196" s="27"/>
-      <c r="I196" s="27"/>
+      <c r="H196" s="30"/>
+      <c r="I196" s="31"/>
       <c r="J196" s="27"/>
       <c r="K196" s="27"/>
       <c r="L196" s="27"/>
@@ -33157,15 +33204,15 @@
       <c r="Y196" s="27"/>
       <c r="Z196" s="27"/>
       <c r="AA196" s="27"/>
-    </row>
-    <row r="197" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C197" s="31"/>
-      <c r="D197" s="31"/>
+      <c r="AB196" s="27"/>
+      <c r="AC196" s="27"/>
+    </row>
+    <row r="197" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E197" s="31"/>
-      <c r="F197" s="30"/>
+      <c r="F197" s="31"/>
       <c r="G197" s="31"/>
-      <c r="H197" s="27"/>
-      <c r="I197" s="27"/>
+      <c r="H197" s="30"/>
+      <c r="I197" s="31"/>
       <c r="J197" s="27"/>
       <c r="K197" s="27"/>
       <c r="L197" s="27"/>
@@ -33184,15 +33231,15 @@
       <c r="Y197" s="27"/>
       <c r="Z197" s="27"/>
       <c r="AA197" s="27"/>
-    </row>
-    <row r="198" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C198" s="31"/>
-      <c r="D198" s="31"/>
+      <c r="AB197" s="27"/>
+      <c r="AC197" s="27"/>
+    </row>
+    <row r="198" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E198" s="31"/>
-      <c r="F198" s="30"/>
+      <c r="F198" s="31"/>
       <c r="G198" s="31"/>
-      <c r="H198" s="27"/>
-      <c r="I198" s="27"/>
+      <c r="H198" s="30"/>
+      <c r="I198" s="31"/>
       <c r="J198" s="27"/>
       <c r="K198" s="27"/>
       <c r="L198" s="27"/>
@@ -33211,15 +33258,15 @@
       <c r="Y198" s="27"/>
       <c r="Z198" s="27"/>
       <c r="AA198" s="27"/>
-    </row>
-    <row r="199" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="C199" s="31"/>
-      <c r="D199" s="31"/>
+      <c r="AB198" s="27"/>
+      <c r="AC198" s="27"/>
+    </row>
+    <row r="199" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E199" s="31"/>
-      <c r="F199" s="30"/>
+      <c r="F199" s="31"/>
       <c r="G199" s="31"/>
-      <c r="H199" s="27"/>
-      <c r="I199" s="27"/>
+      <c r="H199" s="30"/>
+      <c r="I199" s="31"/>
       <c r="J199" s="27"/>
       <c r="K199" s="27"/>
       <c r="L199" s="27"/>
@@ -33238,6 +33285,8 @@
       <c r="Y199" s="27"/>
       <c r="Z199" s="27"/>
       <c r="AA199" s="27"/>
+      <c r="AB199" s="27"/>
+      <c r="AC199" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactor code to catch quantity error, get size, color and add save data to gsheet
</commit_message>
<xml_diff>
--- a/data/order_detail.xlsx
+++ b/data/order_detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\robot_test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC88ECFB-5B61-4BC6-B462-55460F0C0639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE8555B-C989-41D6-9C50-B45B61D1C094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E-commerce Sites" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Supplier Management</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Quantity To Purchase</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Unit Price</t>
   </si>
   <si>
@@ -114,13 +111,35 @@
   <si>
     <t>White</t>
   </si>
+  <si>
+    <t>Min Price</t>
+  </si>
+  <si>
+    <t>Max Price</t>
+  </si>
+  <si>
+    <t>XS, S</t>
+  </si>
+  <si>
+    <t>White, Black</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Jackets</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd&quot;-&quot;mm&quot;-&quot;yyyy&quot; &quot;h&quot;:&quot;mm&quot;:&quot;ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -278,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -361,6 +380,7 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,7 +611,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -634,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -28614,6 +28634,7 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -28622,29 +28643,30 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E989"/>
+  <dimension ref="A1:K989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="34" customWidth="1"/>
     <col min="2" max="2" width="23.140625" style="34" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" style="34" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="34" customWidth="1"/>
-    <col min="6" max="16384" width="12.5703125" style="25"/>
+    <col min="3" max="4" width="34.42578125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="34" customWidth="1"/>
+    <col min="6" max="9" width="25" style="34" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="34" customWidth="1"/>
+    <col min="11" max="16384" width="12.5703125" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="33"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>5</v>
       </c>
@@ -28655,53 +28677,94 @@
         <v>7</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E2" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="986" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J2" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36">
+        <v>45619</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="34">
+        <v>10</v>
+      </c>
+      <c r="H3" s="34">
+        <v>60</v>
+      </c>
+      <c r="I3" s="34">
+        <v>99999999</v>
+      </c>
+    </row>
+    <row r="986" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A986" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E986" s="34">
+      <c r="J986" s="34">
         <v>10</v>
       </c>
     </row>
-    <row r="987" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="987" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A987" s="34" t="s">
         <v>10</v>
       </c>
       <c r="C987" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D987" s="34" t="s">
+      <c r="F987" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E987" s="34">
+      <c r="J987" s="34">
         <v>10</v>
       </c>
     </row>
-    <row r="988" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="988" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A988" s="34" t="s">
         <v>10</v>
       </c>
       <c r="C988" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D988" s="34" t="s">
+      <c r="F988" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E988" s="34">
+      <c r="J988" s="34">
         <v>10</v>
       </c>
     </row>
-    <row r="989" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="989" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C989" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D989" s="34" t="s">
+      <c r="F989" s="34" t="s">
         <v>12</v>
       </c>
     </row>
@@ -28718,8 +28781,8 @@
   </sheetPr>
   <dimension ref="A1:AC199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28775,25 +28838,25 @@
         <v>8</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="22" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
@@ -28818,29 +28881,29 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="35" t="s">
-        <v>29</v>
-      </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3"/>
       <c r="G3">
         <v>45</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" s="28"/>
       <c r="K3" s="27"/>
@@ -33302,7 +33365,7 @@
   <dimension ref="A1:X1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -33315,7 +33378,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="8"/>
@@ -33373,7 +33436,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="10">
         <v>10</v>
@@ -59343,5 +59406,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>